<commit_message>
-Added the new requirements document
-Added the uml diagram
</commit_message>
<xml_diff>
--- a/Docs/lab1/Lab01_ReviewReport.xlsx
+++ b/Docs/lab1/Lab01_ReviewReport.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ptido\Downloads\Tasks_VVSS-master (1)\Tasks_VVSS-master\Docs\lab1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Facultate\VVSS\Tasks\Docs\lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C4D28C-C579-4384-A293-DE344A65D90F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87D4BD4-094B-4682-AF93-4DC4F6DC2E7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -207,9 +207,6 @@
     <t>TaskIO.java/* functions</t>
   </si>
   <si>
-    <t>There are multiple reading/writing functions(a set for binary operations on files, a set of character /string operations for files)</t>
-  </si>
-  <si>
     <t>SonarLint</t>
   </si>
   <si>
@@ -307,6 +304,9 @@
   </si>
   <si>
     <t>1h</t>
+  </si>
+  <si>
+    <t>There are multiple reading/writing functions(a set for binary operations on files, a set of character /string operations for files). Using the wrong function will cause errors in parsing the file.</t>
   </si>
 </sst>
 </file>
@@ -1121,7 +1121,7 @@
         <v>40</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -1130,11 +1130,11 @@
         <v>2</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D11" s="24"/>
       <c r="E11" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -1147,7 +1147,7 @@
       </c>
       <c r="D12" s="24"/>
       <c r="E12" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1276,7 +1276,7 @@
       </c>
       <c r="D27" s="13"/>
       <c r="E27" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1623,7 +1623,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1773,7 +1773,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -1785,7 +1785,7 @@
         <v>57</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -2040,7 +2040,7 @@
         <v>26</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E4" s="39"/>
       <c r="H4" s="18" t="s">
@@ -2103,16 +2103,16 @@
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
@@ -2121,16 +2121,16 @@
         <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -2139,16 +2139,16 @@
         <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
@@ -2157,16 +2157,16 @@
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
@@ -2175,16 +2175,16 @@
         <v>5</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
-Fixed the documentation and fixed issues discovered with SonarLint
</commit_message>
<xml_diff>
--- a/Docs/lab1/Lab01_ReviewReport.xlsx
+++ b/Docs/lab1/Lab01_ReviewReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Facultate\VVSS\Tasks\Docs\lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87D4BD4-094B-4682-AF93-4DC4F6DC2E7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A4D4CCE-676D-469A-A1AC-CEDE2BFB6359}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="86">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -291,22 +291,28 @@
                         }</t>
   </si>
   <si>
-    <t>Incomplete: type of application missing. The application is saving in text and/or binary file?</t>
-  </si>
-  <si>
     <t>R04+R02</t>
   </si>
   <si>
-    <t>Not stated if taks are immediately loaded in when user enters the application</t>
-  </si>
-  <si>
-    <t>JavaFX &amp; JRE required but not specified.</t>
-  </si>
-  <si>
     <t>1h</t>
   </si>
   <si>
     <t>There are multiple reading/writing functions(a set for binary operations on files, a set of character /string operations for files). Using the wrong function will cause errors in parsing the file.</t>
+  </si>
+  <si>
+    <t>Not stated if tasks are immediately loaded in when user enters the application</t>
+  </si>
+  <si>
+    <t>The application is saving in text and/or binary file?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incomplete: type of application missing. </t>
+  </si>
+  <si>
+    <t>R02</t>
+  </si>
+  <si>
+    <t>JavaFX &amp; JRE required but not specified.(and minimum accepted versions)</t>
   </si>
 </sst>
 </file>
@@ -988,15 +994,16 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="141" zoomScaleNormal="141" workbookViewId="0">
-      <selection activeCell="C13" sqref="B13:C13"/>
+    <sheetView zoomScale="141" zoomScaleNormal="141" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="6"/>
     <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" style="6" customWidth="1"/>
     <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
     <col min="6" max="8" width="8.88671875" style="6"/>
     <col min="9" max="9" width="21" style="6" customWidth="1"/>
@@ -1121,7 +1128,7 @@
         <v>40</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -1130,14 +1137,14 @@
         <v>2</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D11" s="24"/>
       <c r="E11" s="23" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
@@ -1147,7 +1154,7 @@
       </c>
       <c r="D12" s="24"/>
       <c r="E12" s="23" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1155,9 +1162,13 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
@@ -1276,7 +1287,7 @@
       </c>
       <c r="D27" s="13"/>
       <c r="E27" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1300,8 +1311,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1622,8 +1633,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1785,7 +1796,7 @@
         <v>57</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1981,8 +1992,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>